<commit_message>
Both created, handled all arround and triggers in database as well
</commit_message>
<xml_diff>
--- a/src/main/resources/pessoal-carga-externa-EXEMPLO.xlsx
+++ b/src/main/resources/pessoal-carga-externa-EXEMPLO.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projeto-golf-invest\golf-commissions\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projeto-golf-invest\golf-data-manager\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0F0B06F-27CF-4233-B2AA-3D78D43C9DA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0D01760-29BD-4636-BFB1-00448DD2DB2F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="90">
   <si>
     <t>Nome</t>
   </si>
@@ -293,7 +293,16 @@
     <t>000.000.000-38</t>
   </si>
   <si>
-    <t>Repasse</t>
+    <t>repasse_prev_assessor</t>
+  </si>
+  <si>
+    <t>repasse_seg_assessor</t>
+  </si>
+  <si>
+    <t>codigo_xerife</t>
+  </si>
+  <si>
+    <t>repasse_prev_xerife</t>
   </si>
 </sst>
 </file>
@@ -671,13 +680,28 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:P45"/>
+  <dimension ref="A1:S45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -694,19 +718,28 @@
         <v>86</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="L1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -727,22 +760,25 @@
       <c r="F2" s="2">
         <v>70</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="2">
+        <v>50</v>
+      </c>
+      <c r="H2">
         <v>341</v>
       </c>
-      <c r="H2" t="str">
+      <c r="I2" t="str">
         <f>A2&amp;A2&amp;A2&amp;A2</f>
         <v>1111</v>
       </c>
-      <c r="I2" t="str">
+      <c r="J2" t="str">
         <f>A2&amp;A2&amp;A2&amp;A2&amp;A2</f>
         <v>11111</v>
       </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -764,26 +800,35 @@
       <c r="F3" s="2">
         <v>70</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="2">
+        <v>50</v>
+      </c>
+      <c r="H3">
         <v>341</v>
       </c>
-      <c r="H3" t="str">
-        <f t="shared" ref="H3:H5" si="1">A3&amp;A3&amp;A3&amp;A3</f>
+      <c r="I3" t="str">
+        <f t="shared" ref="I3:I5" si="1">A3&amp;A3&amp;A3&amp;A3</f>
         <v>2222</v>
       </c>
-      <c r="I3" t="str">
-        <f t="shared" ref="I3:I5" si="2">A3&amp;A3&amp;A3&amp;A3&amp;A3</f>
+      <c r="J3" t="str">
+        <f t="shared" ref="J3:J5" si="2">A3&amp;A3&amp;A3&amp;A3&amp;A3</f>
         <v>22222</v>
       </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M3">
+        <v>10</v>
+      </c>
       <c r="P3" s="3"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4">
         <f t="shared" ref="A4:A40" si="3">A3+1</f>
         <v>3</v>
@@ -805,23 +850,32 @@
       <c r="F4" s="2">
         <v>70</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="2">
+        <v>50</v>
+      </c>
+      <c r="H4">
         <v>341</v>
       </c>
-      <c r="H4" t="str">
+      <c r="I4" t="str">
         <f t="shared" si="1"/>
         <v>3333</v>
       </c>
-      <c r="I4" t="str">
+      <c r="J4" t="str">
         <f t="shared" si="2"/>
         <v>33333</v>
       </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
-      <c r="P4" s="3"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M4">
+        <v>10</v>
+      </c>
+      <c r="S4" s="3"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5">
         <f t="shared" si="3"/>
         <v>4</v>
@@ -843,23 +897,32 @@
       <c r="F5" s="2">
         <v>70</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="2">
+        <v>50</v>
+      </c>
+      <c r="H5">
         <v>341</v>
       </c>
-      <c r="H5" t="str">
+      <c r="I5" t="str">
         <f t="shared" si="1"/>
         <v>4444</v>
       </c>
-      <c r="I5" t="str">
+      <c r="J5" t="str">
         <f t="shared" si="2"/>
         <v>44444</v>
       </c>
-      <c r="J5">
-        <v>1</v>
-      </c>
-      <c r="P5" s="3"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M5">
+        <v>10</v>
+      </c>
+      <c r="S5" s="3"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6">
         <f t="shared" si="3"/>
         <v>5</v>
@@ -881,23 +944,32 @@
       <c r="F6" s="2">
         <v>70</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="2">
+        <v>50</v>
+      </c>
+      <c r="H6">
         <v>341</v>
       </c>
-      <c r="H6" t="str">
+      <c r="I6" t="str">
         <f>A6&amp;A6&amp;A6&amp;A6</f>
         <v>5555</v>
       </c>
-      <c r="I6" t="str">
+      <c r="J6" t="str">
         <f>A6&amp;A6&amp;A6&amp;A6&amp;A6</f>
         <v>55555</v>
       </c>
-      <c r="J6">
-        <v>1</v>
-      </c>
-      <c r="P6" s="3"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M6">
+        <v>10</v>
+      </c>
+      <c r="S6" s="3"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7">
         <f t="shared" si="3"/>
         <v>6</v>
@@ -919,23 +991,32 @@
       <c r="F7" s="2">
         <v>70</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="2">
+        <v>50</v>
+      </c>
+      <c r="H7">
         <v>341</v>
       </c>
-      <c r="H7" t="str">
-        <f t="shared" ref="H7:H10" si="5">A7&amp;A7&amp;A7&amp;A7</f>
+      <c r="I7" t="str">
+        <f t="shared" ref="I7:I10" si="5">A7&amp;A7&amp;A7&amp;A7</f>
         <v>6666</v>
       </c>
-      <c r="I7" t="str">
-        <f t="shared" ref="I7:I10" si="6">A7&amp;A7&amp;A7&amp;A7&amp;A7</f>
+      <c r="J7" t="str">
+        <f t="shared" ref="J7:J10" si="6">A7&amp;A7&amp;A7&amp;A7&amp;A7</f>
         <v>66666</v>
       </c>
-      <c r="J7">
-        <v>1</v>
-      </c>
-      <c r="P7" s="3"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M7">
+        <v>10</v>
+      </c>
+      <c r="S7" s="3"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8">
         <f t="shared" si="3"/>
         <v>7</v>
@@ -957,23 +1038,32 @@
       <c r="F8" s="2">
         <v>70</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="2">
+        <v>50</v>
+      </c>
+      <c r="H8">
         <v>341</v>
       </c>
-      <c r="H8" t="str">
+      <c r="I8" t="str">
         <f t="shared" si="5"/>
         <v>7777</v>
       </c>
-      <c r="I8" t="str">
+      <c r="J8" t="str">
         <f t="shared" si="6"/>
         <v>77777</v>
       </c>
-      <c r="J8">
-        <v>1</v>
-      </c>
-      <c r="P8" s="3"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M8">
+        <v>10</v>
+      </c>
+      <c r="S8" s="3"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9">
         <f t="shared" si="3"/>
         <v>8</v>
@@ -995,23 +1085,32 @@
       <c r="F9" s="2">
         <v>70</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="2">
+        <v>50</v>
+      </c>
+      <c r="H9">
         <v>341</v>
       </c>
-      <c r="H9" t="str">
+      <c r="I9" t="str">
         <f t="shared" si="5"/>
         <v>8888</v>
       </c>
-      <c r="I9" t="str">
+      <c r="J9" t="str">
         <f t="shared" si="6"/>
         <v>88888</v>
       </c>
-      <c r="J9">
-        <v>1</v>
-      </c>
-      <c r="P9" s="3"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M9">
+        <v>10</v>
+      </c>
+      <c r="S9" s="3"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10">
         <f t="shared" si="3"/>
         <v>9</v>
@@ -1033,23 +1132,32 @@
       <c r="F10" s="2">
         <v>70</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="2">
+        <v>50</v>
+      </c>
+      <c r="H10">
         <v>341</v>
       </c>
-      <c r="H10" t="str">
+      <c r="I10" t="str">
         <f t="shared" si="5"/>
         <v>9999</v>
       </c>
-      <c r="I10" t="str">
+      <c r="J10" t="str">
         <f t="shared" si="6"/>
         <v>99999</v>
       </c>
-      <c r="J10">
-        <v>1</v>
-      </c>
-      <c r="P10" s="3"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M10">
+        <v>10</v>
+      </c>
+      <c r="S10" s="3"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11">
         <f t="shared" si="3"/>
         <v>10</v>
@@ -1069,25 +1177,34 @@
         <v>17</v>
       </c>
       <c r="F11" s="2">
-        <v>70</v>
-      </c>
-      <c r="G11">
+        <v>65</v>
+      </c>
+      <c r="G11" s="2">
+        <v>45</v>
+      </c>
+      <c r="H11">
         <v>341</v>
       </c>
-      <c r="H11" t="str">
+      <c r="I11" t="str">
         <f>A11&amp;A11</f>
         <v>1010</v>
       </c>
-      <c r="I11" t="str">
+      <c r="J11" t="str">
         <f>A11&amp;A11&amp;A11</f>
         <v>101010</v>
       </c>
-      <c r="J11">
-        <v>1</v>
-      </c>
-      <c r="P11" s="3"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M11">
+        <v>10</v>
+      </c>
+      <c r="S11" s="3"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12">
         <f t="shared" si="3"/>
         <v>11</v>
@@ -1107,25 +1224,34 @@
         <v>18</v>
       </c>
       <c r="F12" s="2">
-        <v>70</v>
-      </c>
-      <c r="G12">
+        <v>65</v>
+      </c>
+      <c r="G12" s="2">
+        <v>45</v>
+      </c>
+      <c r="H12">
         <v>341</v>
       </c>
-      <c r="H12" t="str">
-        <f t="shared" ref="H12:H40" si="7">A12&amp;A12</f>
+      <c r="I12" t="str">
+        <f t="shared" ref="I12:I40" si="7">A12&amp;A12</f>
         <v>1111</v>
       </c>
-      <c r="I12" t="str">
-        <f t="shared" ref="I12:I40" si="8">A12&amp;A12&amp;A12</f>
+      <c r="J12" t="str">
+        <f t="shared" ref="J12:J40" si="8">A12&amp;A12&amp;A12</f>
         <v>111111</v>
       </c>
-      <c r="J12">
-        <v>1</v>
-      </c>
-      <c r="P12" s="3"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M12">
+        <v>10</v>
+      </c>
+      <c r="S12" s="3"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13">
         <f t="shared" si="3"/>
         <v>12</v>
@@ -1145,25 +1271,34 @@
         <v>19</v>
       </c>
       <c r="F13" s="2">
-        <v>70</v>
-      </c>
-      <c r="G13">
+        <v>65</v>
+      </c>
+      <c r="G13" s="2">
+        <v>45</v>
+      </c>
+      <c r="H13">
         <v>341</v>
       </c>
-      <c r="H13" t="str">
+      <c r="I13" t="str">
         <f t="shared" si="7"/>
         <v>1212</v>
       </c>
-      <c r="I13" t="str">
+      <c r="J13" t="str">
         <f t="shared" si="8"/>
         <v>121212</v>
       </c>
-      <c r="J13">
-        <v>1</v>
-      </c>
-      <c r="P13" s="3"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M13">
+        <v>10</v>
+      </c>
+      <c r="S13" s="3"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14">
         <f t="shared" si="3"/>
         <v>13</v>
@@ -1183,25 +1318,34 @@
         <v>20</v>
       </c>
       <c r="F14" s="2">
-        <v>70</v>
-      </c>
-      <c r="G14">
+        <v>65</v>
+      </c>
+      <c r="G14" s="2">
+        <v>45</v>
+      </c>
+      <c r="H14">
         <v>341</v>
       </c>
-      <c r="H14" t="str">
+      <c r="I14" t="str">
         <f t="shared" si="7"/>
         <v>1313</v>
       </c>
-      <c r="I14" t="str">
+      <c r="J14" t="str">
         <f t="shared" si="8"/>
         <v>131313</v>
       </c>
-      <c r="J14">
-        <v>1</v>
-      </c>
-      <c r="P14" s="3"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M14">
+        <v>10</v>
+      </c>
+      <c r="S14" s="3"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15">
         <f t="shared" si="3"/>
         <v>14</v>
@@ -1221,25 +1365,34 @@
         <v>21</v>
       </c>
       <c r="F15" s="2">
-        <v>70</v>
-      </c>
-      <c r="G15">
+        <v>65</v>
+      </c>
+      <c r="G15" s="2">
+        <v>45</v>
+      </c>
+      <c r="H15">
         <v>341</v>
       </c>
-      <c r="H15" t="str">
+      <c r="I15" t="str">
         <f t="shared" si="7"/>
         <v>1414</v>
       </c>
-      <c r="I15" t="str">
+      <c r="J15" t="str">
         <f t="shared" si="8"/>
         <v>141414</v>
       </c>
-      <c r="J15">
-        <v>1</v>
-      </c>
-      <c r="P15" s="3"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M15">
+        <v>10</v>
+      </c>
+      <c r="S15" s="3"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16">
         <f t="shared" si="3"/>
         <v>15</v>
@@ -1259,25 +1412,34 @@
         <v>22</v>
       </c>
       <c r="F16" s="2">
-        <v>70</v>
-      </c>
-      <c r="G16">
+        <v>65</v>
+      </c>
+      <c r="G16" s="2">
+        <v>45</v>
+      </c>
+      <c r="H16">
         <v>341</v>
       </c>
-      <c r="H16" t="str">
+      <c r="I16" t="str">
         <f t="shared" si="7"/>
         <v>1515</v>
       </c>
-      <c r="I16" t="str">
+      <c r="J16" t="str">
         <f t="shared" si="8"/>
         <v>151515</v>
       </c>
-      <c r="J16">
-        <v>1</v>
-      </c>
-      <c r="P16" s="3"/>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K16">
+        <v>1</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M16">
+        <v>10</v>
+      </c>
+      <c r="S16" s="3"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17">
         <f t="shared" si="3"/>
         <v>16</v>
@@ -1297,25 +1459,34 @@
         <v>23</v>
       </c>
       <c r="F17" s="2">
-        <v>70</v>
-      </c>
-      <c r="G17">
+        <v>65</v>
+      </c>
+      <c r="G17" s="2">
+        <v>45</v>
+      </c>
+      <c r="H17">
         <v>341</v>
       </c>
-      <c r="H17" t="str">
+      <c r="I17" t="str">
         <f t="shared" si="7"/>
         <v>1616</v>
       </c>
-      <c r="I17" t="str">
+      <c r="J17" t="str">
         <f t="shared" si="8"/>
         <v>161616</v>
       </c>
-      <c r="J17">
-        <v>1</v>
-      </c>
-      <c r="P17" s="3"/>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M17">
+        <v>10</v>
+      </c>
+      <c r="S17" s="3"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18">
         <f t="shared" si="3"/>
         <v>17</v>
@@ -1335,25 +1506,34 @@
         <v>24</v>
       </c>
       <c r="F18" s="2">
-        <v>70</v>
-      </c>
-      <c r="G18">
+        <v>65</v>
+      </c>
+      <c r="G18" s="2">
+        <v>45</v>
+      </c>
+      <c r="H18">
         <v>341</v>
       </c>
-      <c r="H18" t="str">
+      <c r="I18" t="str">
         <f t="shared" si="7"/>
         <v>1717</v>
       </c>
-      <c r="I18" t="str">
+      <c r="J18" t="str">
         <f t="shared" si="8"/>
         <v>171717</v>
       </c>
-      <c r="J18">
-        <v>1</v>
-      </c>
-      <c r="P18" s="3"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M18">
+        <v>10</v>
+      </c>
+      <c r="S18" s="3"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19">
         <f t="shared" si="3"/>
         <v>18</v>
@@ -1373,25 +1553,34 @@
         <v>25</v>
       </c>
       <c r="F19" s="2">
-        <v>70</v>
-      </c>
-      <c r="G19">
+        <v>65</v>
+      </c>
+      <c r="G19" s="2">
+        <v>45</v>
+      </c>
+      <c r="H19">
         <v>341</v>
       </c>
-      <c r="H19" t="str">
+      <c r="I19" t="str">
         <f t="shared" si="7"/>
         <v>1818</v>
       </c>
-      <c r="I19" t="str">
+      <c r="J19" t="str">
         <f t="shared" si="8"/>
         <v>181818</v>
       </c>
-      <c r="J19">
-        <v>1</v>
-      </c>
-      <c r="P19" s="3"/>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K19">
+        <v>1</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M19">
+        <v>10</v>
+      </c>
+      <c r="S19" s="3"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20">
         <f t="shared" si="3"/>
         <v>19</v>
@@ -1411,25 +1600,34 @@
         <v>26</v>
       </c>
       <c r="F20" s="2">
-        <v>70</v>
-      </c>
-      <c r="G20">
+        <v>65</v>
+      </c>
+      <c r="G20" s="2">
+        <v>45</v>
+      </c>
+      <c r="H20">
         <v>341</v>
       </c>
-      <c r="H20" t="str">
+      <c r="I20" t="str">
         <f t="shared" si="7"/>
         <v>1919</v>
       </c>
-      <c r="I20" t="str">
+      <c r="J20" t="str">
         <f t="shared" si="8"/>
         <v>191919</v>
       </c>
-      <c r="J20">
-        <v>1</v>
-      </c>
-      <c r="P20" s="3"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K20">
+        <v>1</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M20">
+        <v>10</v>
+      </c>
+      <c r="S20" s="3"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21">
         <f t="shared" si="3"/>
         <v>20</v>
@@ -1449,25 +1647,34 @@
         <v>27</v>
       </c>
       <c r="F21" s="2">
-        <v>70</v>
-      </c>
-      <c r="G21">
+        <v>65</v>
+      </c>
+      <c r="G21" s="2">
+        <v>45</v>
+      </c>
+      <c r="H21">
         <v>341</v>
       </c>
-      <c r="H21" t="str">
+      <c r="I21" t="str">
         <f t="shared" si="7"/>
         <v>2020</v>
       </c>
-      <c r="I21" t="str">
+      <c r="J21" t="str">
         <f t="shared" si="8"/>
         <v>202020</v>
       </c>
-      <c r="J21">
-        <v>1</v>
-      </c>
-      <c r="P21" s="3"/>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K21">
+        <v>1</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M21">
+        <v>10</v>
+      </c>
+      <c r="S21" s="3"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22">
         <f t="shared" si="3"/>
         <v>21</v>
@@ -1487,25 +1694,34 @@
         <v>28</v>
       </c>
       <c r="F22" s="2">
-        <v>70</v>
-      </c>
-      <c r="G22">
+        <v>65</v>
+      </c>
+      <c r="G22" s="2">
+        <v>45</v>
+      </c>
+      <c r="H22">
         <v>353</v>
       </c>
-      <c r="H22" t="str">
+      <c r="I22" t="str">
         <f t="shared" si="7"/>
         <v>2121</v>
       </c>
-      <c r="I22" t="str">
+      <c r="J22" t="str">
         <f t="shared" si="8"/>
         <v>212121</v>
       </c>
-      <c r="J22">
-        <v>1</v>
-      </c>
-      <c r="P22" s="3"/>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K22">
+        <v>1</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M22">
+        <v>10</v>
+      </c>
+      <c r="S22" s="3"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23">
         <f t="shared" si="3"/>
         <v>22</v>
@@ -1525,25 +1741,34 @@
         <v>29</v>
       </c>
       <c r="F23" s="2">
-        <v>70</v>
-      </c>
-      <c r="G23">
+        <v>65</v>
+      </c>
+      <c r="G23" s="2">
+        <v>45</v>
+      </c>
+      <c r="H23">
         <v>354</v>
       </c>
-      <c r="H23" t="str">
+      <c r="I23" t="str">
         <f t="shared" si="7"/>
         <v>2222</v>
       </c>
-      <c r="I23" t="str">
+      <c r="J23" t="str">
         <f t="shared" si="8"/>
         <v>222222</v>
       </c>
-      <c r="J23">
-        <v>1</v>
-      </c>
-      <c r="P23" s="3"/>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K23">
+        <v>1</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M23">
+        <v>10</v>
+      </c>
+      <c r="S23" s="3"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24">
         <f t="shared" si="3"/>
         <v>23</v>
@@ -1563,25 +1788,34 @@
         <v>30</v>
       </c>
       <c r="F24" s="2">
-        <v>70</v>
-      </c>
-      <c r="G24">
+        <v>65</v>
+      </c>
+      <c r="G24" s="2">
+        <v>45</v>
+      </c>
+      <c r="H24">
         <v>355</v>
       </c>
-      <c r="H24" t="str">
+      <c r="I24" t="str">
         <f t="shared" si="7"/>
         <v>2323</v>
       </c>
-      <c r="I24" t="str">
+      <c r="J24" t="str">
         <f t="shared" si="8"/>
         <v>232323</v>
       </c>
-      <c r="J24">
-        <v>1</v>
-      </c>
-      <c r="P24" s="3"/>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K24">
+        <v>1</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M24">
+        <v>10</v>
+      </c>
+      <c r="S24" s="3"/>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25">
         <f t="shared" si="3"/>
         <v>24</v>
@@ -1601,25 +1835,34 @@
         <v>31</v>
       </c>
       <c r="F25" s="2">
-        <v>70</v>
-      </c>
-      <c r="G25">
+        <v>60</v>
+      </c>
+      <c r="G25" s="2">
+        <v>40</v>
+      </c>
+      <c r="H25">
         <v>356</v>
       </c>
-      <c r="H25" t="str">
+      <c r="I25" t="str">
         <f t="shared" si="7"/>
         <v>2424</v>
       </c>
-      <c r="I25" t="str">
+      <c r="J25" t="str">
         <f t="shared" si="8"/>
         <v>242424</v>
       </c>
-      <c r="J25">
-        <v>1</v>
-      </c>
-      <c r="P25" s="3"/>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K25">
+        <v>1</v>
+      </c>
+      <c r="L25" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M25">
+        <v>10</v>
+      </c>
+      <c r="S25" s="3"/>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26">
         <f t="shared" si="3"/>
         <v>25</v>
@@ -1639,25 +1882,34 @@
         <v>32</v>
       </c>
       <c r="F26" s="2">
-        <v>70</v>
-      </c>
-      <c r="G26">
+        <v>60</v>
+      </c>
+      <c r="G26" s="2">
+        <v>40</v>
+      </c>
+      <c r="H26">
         <v>357</v>
       </c>
-      <c r="H26" t="str">
+      <c r="I26" t="str">
         <f t="shared" si="7"/>
         <v>2525</v>
       </c>
-      <c r="I26" t="str">
+      <c r="J26" t="str">
         <f t="shared" si="8"/>
         <v>252525</v>
       </c>
-      <c r="J26">
-        <v>1</v>
-      </c>
-      <c r="P26" s="3"/>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K26">
+        <v>1</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M26">
+        <v>10</v>
+      </c>
+      <c r="S26" s="3"/>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27">
         <f t="shared" si="3"/>
         <v>26</v>
@@ -1677,25 +1929,34 @@
         <v>33</v>
       </c>
       <c r="F27" s="2">
-        <v>70</v>
-      </c>
-      <c r="G27">
+        <v>60</v>
+      </c>
+      <c r="G27" s="2">
+        <v>40</v>
+      </c>
+      <c r="H27">
         <v>358</v>
       </c>
-      <c r="H27" t="str">
+      <c r="I27" t="str">
         <f t="shared" si="7"/>
         <v>2626</v>
       </c>
-      <c r="I27" t="str">
+      <c r="J27" t="str">
         <f t="shared" si="8"/>
         <v>262626</v>
       </c>
-      <c r="J27">
-        <v>1</v>
-      </c>
-      <c r="P27" s="3"/>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K27">
+        <v>1</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M27">
+        <v>10</v>
+      </c>
+      <c r="S27" s="3"/>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28">
         <f t="shared" si="3"/>
         <v>27</v>
@@ -1715,25 +1976,34 @@
         <v>34</v>
       </c>
       <c r="F28" s="2">
-        <v>70</v>
-      </c>
-      <c r="G28">
+        <v>60</v>
+      </c>
+      <c r="G28" s="2">
+        <v>40</v>
+      </c>
+      <c r="H28">
         <v>359</v>
       </c>
-      <c r="H28" t="str">
+      <c r="I28" t="str">
         <f t="shared" si="7"/>
         <v>2727</v>
       </c>
-      <c r="I28" t="str">
+      <c r="J28" t="str">
         <f t="shared" si="8"/>
         <v>272727</v>
       </c>
-      <c r="J28">
-        <v>1</v>
-      </c>
-      <c r="P28" s="3"/>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K28">
+        <v>1</v>
+      </c>
+      <c r="L28" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M28">
+        <v>10</v>
+      </c>
+      <c r="S28" s="3"/>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29">
         <f t="shared" si="3"/>
         <v>28</v>
@@ -1753,25 +2023,34 @@
         <v>35</v>
       </c>
       <c r="F29" s="2">
-        <v>70</v>
-      </c>
-      <c r="G29">
+        <v>60</v>
+      </c>
+      <c r="G29" s="2">
+        <v>40</v>
+      </c>
+      <c r="H29">
         <v>360</v>
       </c>
-      <c r="H29" t="str">
+      <c r="I29" t="str">
         <f t="shared" si="7"/>
         <v>2828</v>
       </c>
-      <c r="I29" t="str">
+      <c r="J29" t="str">
         <f t="shared" si="8"/>
         <v>282828</v>
       </c>
-      <c r="J29">
-        <v>1</v>
-      </c>
-      <c r="P29" s="3"/>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K29">
+        <v>1</v>
+      </c>
+      <c r="L29" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M29">
+        <v>10</v>
+      </c>
+      <c r="S29" s="3"/>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30">
         <f t="shared" si="3"/>
         <v>29</v>
@@ -1791,25 +2070,34 @@
         <v>36</v>
       </c>
       <c r="F30" s="2">
-        <v>70</v>
-      </c>
-      <c r="G30">
+        <v>60</v>
+      </c>
+      <c r="G30" s="2">
+        <v>40</v>
+      </c>
+      <c r="H30">
         <v>361</v>
       </c>
-      <c r="H30" t="str">
+      <c r="I30" t="str">
         <f t="shared" si="7"/>
         <v>2929</v>
       </c>
-      <c r="I30" t="str">
+      <c r="J30" t="str">
         <f t="shared" si="8"/>
         <v>292929</v>
       </c>
-      <c r="J30">
-        <v>1</v>
-      </c>
-      <c r="P30" s="3"/>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K30">
+        <v>1</v>
+      </c>
+      <c r="L30" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M30">
+        <v>10</v>
+      </c>
+      <c r="S30" s="3"/>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31">
         <f t="shared" si="3"/>
         <v>30</v>
@@ -1829,25 +2117,34 @@
         <v>37</v>
       </c>
       <c r="F31" s="2">
-        <v>70</v>
-      </c>
-      <c r="G31">
+        <v>60</v>
+      </c>
+      <c r="G31" s="2">
+        <v>40</v>
+      </c>
+      <c r="H31">
         <v>362</v>
       </c>
-      <c r="H31" t="str">
+      <c r="I31" t="str">
         <f t="shared" si="7"/>
         <v>3030</v>
       </c>
-      <c r="I31" t="str">
+      <c r="J31" t="str">
         <f t="shared" si="8"/>
         <v>303030</v>
       </c>
-      <c r="J31">
-        <v>1</v>
-      </c>
-      <c r="P31" s="3"/>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K31">
+        <v>1</v>
+      </c>
+      <c r="L31" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M31">
+        <v>10</v>
+      </c>
+      <c r="S31" s="3"/>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32">
         <f t="shared" si="3"/>
         <v>31</v>
@@ -1867,25 +2164,34 @@
         <v>38</v>
       </c>
       <c r="F32" s="2">
-        <v>70</v>
-      </c>
-      <c r="G32">
+        <v>60</v>
+      </c>
+      <c r="G32" s="2">
+        <v>40</v>
+      </c>
+      <c r="H32">
         <v>363</v>
       </c>
-      <c r="H32" t="str">
+      <c r="I32" t="str">
         <f t="shared" si="7"/>
         <v>3131</v>
       </c>
-      <c r="I32" t="str">
+      <c r="J32" t="str">
         <f t="shared" si="8"/>
         <v>313131</v>
       </c>
-      <c r="J32">
-        <v>1</v>
-      </c>
-      <c r="P32" s="3"/>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K32">
+        <v>1</v>
+      </c>
+      <c r="L32" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M32">
+        <v>10</v>
+      </c>
+      <c r="S32" s="3"/>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A33">
         <f t="shared" si="3"/>
         <v>32</v>
@@ -1905,25 +2211,34 @@
         <v>39</v>
       </c>
       <c r="F33" s="2">
-        <v>70</v>
-      </c>
-      <c r="G33">
+        <v>60</v>
+      </c>
+      <c r="G33" s="2">
+        <v>40</v>
+      </c>
+      <c r="H33">
         <v>364</v>
       </c>
-      <c r="H33" t="str">
+      <c r="I33" t="str">
         <f t="shared" si="7"/>
         <v>3232</v>
       </c>
-      <c r="I33" t="str">
+      <c r="J33" t="str">
         <f t="shared" si="8"/>
         <v>323232</v>
       </c>
-      <c r="J33">
-        <v>1</v>
-      </c>
-      <c r="P33" s="3"/>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K33">
+        <v>1</v>
+      </c>
+      <c r="L33" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M33">
+        <v>10</v>
+      </c>
+      <c r="S33" s="3"/>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A34">
         <f t="shared" si="3"/>
         <v>33</v>
@@ -1943,25 +2258,34 @@
         <v>40</v>
       </c>
       <c r="F34" s="2">
-        <v>70</v>
-      </c>
-      <c r="G34">
+        <v>60</v>
+      </c>
+      <c r="G34" s="2">
+        <v>40</v>
+      </c>
+      <c r="H34">
         <v>365</v>
       </c>
-      <c r="H34" t="str">
+      <c r="I34" t="str">
         <f t="shared" si="7"/>
         <v>3333</v>
       </c>
-      <c r="I34" t="str">
+      <c r="J34" t="str">
         <f t="shared" si="8"/>
         <v>333333</v>
       </c>
-      <c r="J34">
-        <v>1</v>
-      </c>
-      <c r="P34" s="3"/>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K34">
+        <v>1</v>
+      </c>
+      <c r="L34" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M34">
+        <v>10</v>
+      </c>
+      <c r="S34" s="3"/>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A35">
         <f t="shared" si="3"/>
         <v>34</v>
@@ -1981,25 +2305,34 @@
         <v>41</v>
       </c>
       <c r="F35" s="2">
-        <v>70</v>
-      </c>
-      <c r="G35">
+        <v>60</v>
+      </c>
+      <c r="G35" s="2">
+        <v>40</v>
+      </c>
+      <c r="H35">
         <v>366</v>
       </c>
-      <c r="H35" t="str">
+      <c r="I35" t="str">
         <f t="shared" si="7"/>
         <v>3434</v>
       </c>
-      <c r="I35" t="str">
+      <c r="J35" t="str">
         <f t="shared" si="8"/>
         <v>343434</v>
       </c>
-      <c r="J35">
-        <v>1</v>
-      </c>
-      <c r="P35" s="3"/>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K35">
+        <v>1</v>
+      </c>
+      <c r="L35" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M35">
+        <v>10</v>
+      </c>
+      <c r="S35" s="3"/>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A36">
         <f t="shared" si="3"/>
         <v>35</v>
@@ -2019,25 +2352,34 @@
         <v>42</v>
       </c>
       <c r="F36" s="2">
-        <v>70</v>
-      </c>
-      <c r="G36">
+        <v>60</v>
+      </c>
+      <c r="G36" s="2">
+        <v>40</v>
+      </c>
+      <c r="H36">
         <v>367</v>
       </c>
-      <c r="H36" t="str">
+      <c r="I36" t="str">
         <f t="shared" si="7"/>
         <v>3535</v>
       </c>
-      <c r="I36" t="str">
+      <c r="J36" t="str">
         <f t="shared" si="8"/>
         <v>353535</v>
       </c>
-      <c r="J36">
-        <v>1</v>
-      </c>
-      <c r="P36" s="3"/>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K36">
+        <v>1</v>
+      </c>
+      <c r="L36" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M36">
+        <v>10</v>
+      </c>
+      <c r="S36" s="3"/>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A37">
         <f t="shared" si="3"/>
         <v>36</v>
@@ -2057,25 +2399,34 @@
         <v>43</v>
       </c>
       <c r="F37" s="2">
-        <v>70</v>
-      </c>
-      <c r="G37">
+        <v>60</v>
+      </c>
+      <c r="G37" s="2">
+        <v>40</v>
+      </c>
+      <c r="H37">
         <v>368</v>
       </c>
-      <c r="H37" t="str">
+      <c r="I37" t="str">
         <f t="shared" si="7"/>
         <v>3636</v>
       </c>
-      <c r="I37" t="str">
+      <c r="J37" t="str">
         <f t="shared" si="8"/>
         <v>363636</v>
       </c>
-      <c r="J37">
-        <v>1</v>
-      </c>
-      <c r="P37" s="3"/>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K37">
+        <v>1</v>
+      </c>
+      <c r="L37" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M37">
+        <v>10</v>
+      </c>
+      <c r="S37" s="3"/>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A38">
         <f t="shared" si="3"/>
         <v>37</v>
@@ -2095,25 +2446,34 @@
         <v>44</v>
       </c>
       <c r="F38" s="2">
-        <v>70</v>
-      </c>
-      <c r="G38">
+        <v>60</v>
+      </c>
+      <c r="G38" s="2">
+        <v>40</v>
+      </c>
+      <c r="H38">
         <v>369</v>
       </c>
-      <c r="H38" t="str">
+      <c r="I38" t="str">
         <f t="shared" si="7"/>
         <v>3737</v>
       </c>
-      <c r="I38" t="str">
+      <c r="J38" t="str">
         <f t="shared" si="8"/>
         <v>373737</v>
       </c>
-      <c r="J38">
-        <v>1</v>
-      </c>
-      <c r="P38" s="3"/>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K38">
+        <v>1</v>
+      </c>
+      <c r="L38" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M38">
+        <v>10</v>
+      </c>
+      <c r="S38" s="3"/>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A39">
         <f t="shared" si="3"/>
         <v>38</v>
@@ -2133,25 +2493,34 @@
         <v>45</v>
       </c>
       <c r="F39" s="2">
-        <v>70</v>
-      </c>
-      <c r="G39">
+        <v>60</v>
+      </c>
+      <c r="G39" s="2">
+        <v>40</v>
+      </c>
+      <c r="H39">
         <v>370</v>
       </c>
-      <c r="H39" t="str">
+      <c r="I39" t="str">
         <f t="shared" si="7"/>
         <v>3838</v>
       </c>
-      <c r="I39" t="str">
+      <c r="J39" t="str">
         <f t="shared" si="8"/>
         <v>383838</v>
       </c>
-      <c r="J39">
-        <v>1</v>
-      </c>
-      <c r="P39" s="3"/>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K39">
+        <v>1</v>
+      </c>
+      <c r="L39" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M39">
+        <v>10</v>
+      </c>
+      <c r="S39" s="3"/>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A40">
         <f t="shared" si="3"/>
         <v>39</v>
@@ -2171,38 +2540,47 @@
         <v>46</v>
       </c>
       <c r="F40" s="2">
-        <v>70</v>
-      </c>
-      <c r="G40">
+        <v>60</v>
+      </c>
+      <c r="G40" s="2">
+        <v>40</v>
+      </c>
+      <c r="H40">
         <v>371</v>
       </c>
-      <c r="H40" t="str">
+      <c r="I40" t="str">
         <f t="shared" si="7"/>
         <v>3939</v>
       </c>
-      <c r="I40" t="str">
+      <c r="J40" t="str">
         <f t="shared" si="8"/>
         <v>393939</v>
       </c>
-      <c r="J40">
-        <v>1</v>
-      </c>
-      <c r="P40" s="3"/>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="P41" s="3"/>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="P42" s="3"/>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="P43" s="3"/>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="P44" s="3"/>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="P45" s="3"/>
+      <c r="K40">
+        <v>1</v>
+      </c>
+      <c r="L40" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M40">
+        <v>10</v>
+      </c>
+      <c r="S40" s="3"/>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S41" s="3"/>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S42" s="3"/>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S43" s="3"/>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S44" s="3"/>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S45" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>